<commit_message>
RDM-9555: Definition Store Changes for Conditional Event Post State
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_NOC_CONFIG.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_NOC_CONFIG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B8B819-E135-C34C-BDDE-32E76BF9B145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC4AC48-AEF3-584E-8CAB-32D8EAE377A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35200" windowHeight="19700" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35200" windowHeight="19700" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="374">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1190,6 +1190,15 @@
   </si>
   <si>
     <t>NoticeOfChangeConfig</t>
+  </si>
+  <si>
+    <t>*(PersonHasSecondAddress="Yes"):1;CaseStopped</t>
+  </si>
+  <si>
+    <t>CaseEnteredIntoLegacy(PersonHasSecondAddress="Last"):1;CaseStopped</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -1846,7 +1855,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="213">
+  <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -2144,6 +2153,7 @@
     <xf numFmtId="49" fontId="49" fillId="4" borderId="22" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -15601,7 +15611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E882E8-CCDE-8C41-B416-088AC35BA427}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+    <sheetView zoomScale="112" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -15669,8 +15679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -16917,17 +16927,29 @@
       <c r="W32" s="26"/>
     </row>
     <row r="33" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="9"/>
+      <c r="A33" s="27">
+        <v>42736</v>
+      </c>
       <c r="B33" s="9"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="C33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>57</v>
+      </c>
       <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="G33" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
+      <c r="K33" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
@@ -18888,7 +18910,7 @@
   <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:E3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -18901,7 +18923,7 @@
     <col min="6" max="6" width="45.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="45.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="61.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29.6640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="32" style="1" customWidth="1"/>
     <col min="12" max="12" width="31.33203125" style="1" customWidth="1"/>
@@ -19091,7 +19113,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="4"/>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="213" t="s">
         <v>145</v>
       </c>
       <c r="J4" s="41" t="s">
@@ -19144,8 +19166,8 @@
       <c r="H5" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>147</v>
+      <c r="I5" s="213" t="s">
+        <v>371</v>
       </c>
       <c r="J5" s="41"/>
       <c r="K5" s="41"/>
@@ -19191,7 +19213,7 @@
       <c r="H6" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="213" t="s">
         <v>149</v>
       </c>
       <c r="J6" s="41"/>
@@ -19232,7 +19254,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="213" t="s">
         <v>145</v>
       </c>
       <c r="J7" s="41"/>
@@ -19277,8 +19299,8 @@
       <c r="H8" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>147</v>
+      <c r="I8" s="213" t="s">
+        <v>372</v>
       </c>
       <c r="J8" s="41"/>
       <c r="K8" s="41"/>
@@ -19322,8 +19344,8 @@
       <c r="H9" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>149</v>
+      <c r="I9" s="213" t="s">
+        <v>373</v>
       </c>
       <c r="J9" s="41"/>
       <c r="K9" s="41"/>

</xml_diff>